<commit_message>
fix a mistake when counting adds in vertexInterp
</commit_message>
<xml_diff>
--- a/Data/baseline_timing.xlsx
+++ b/Data/baseline_timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eth\asl\team42\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6350D54-9723-4B45-BEB6-75C529BBEA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B730ACD3-6AEF-4892-AF01-6FCF25015E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1F9DB3D-A5ED-4CF3-8993-B9AA5F6B7807}"/>
   </bookViews>
@@ -547,34 +547,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.49748347858856862</c:v>
+                  <c:v>0.41592563416263895</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39495470769115798</c:v>
+                  <c:v>0.34059010718292138</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33688794262014748</c:v>
+                  <c:v>0.2970727219302598</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31416074310012626</c:v>
+                  <c:v>0.28098741734431881</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.29461369017176064</c:v>
+                  <c:v>0.26671040093023402</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27888171284255747</c:v>
+                  <c:v>0.25509964508497446</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26503320751336201</c:v>
+                  <c:v>0.24433633305120112</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25505175736398827</c:v>
+                  <c:v>0.23666255606934924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.24647103627791317</c:v>
+                  <c:v>0.23009253625401557</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2399613090061532</c:v>
+                  <c:v>0.22503445058759797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,34 +670,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.20779247932833639</c:v>
+                  <c:v>0.20435157350689198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19008113507889787</c:v>
+                  <c:v>0.18903218651325307</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19620276958603941</c:v>
+                  <c:v>0.19505971752458229</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19475661614713657</c:v>
+                  <c:v>0.19418922833756871</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19591126502897765</c:v>
+                  <c:v>0.19532763977043302</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.19501287501118031</c:v>
+                  <c:v>0.19471428504178578</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.19518225405811335</c:v>
+                  <c:v>0.19480691115616602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.19439825946692643</c:v>
+                  <c:v>0.19408299736292856</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.19491339731850818</c:v>
+                  <c:v>0.19458412618878609</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19358716310804974</c:v>
+                  <c:v>0.19334298037912881</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -745,7 +745,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -758,10 +758,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1050"/>
                   <a:t>MC grid resolution</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1050"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -778,7 +778,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -952,8 +952,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72448671887325566"/>
-          <c:y val="0.47425420907752391"/>
+          <c:x val="0.72448676919770993"/>
+          <c:y val="0.40989106544608761"/>
           <c:w val="0.24363714269322892"/>
           <c:h val="0.32774470264387684"/>
         </c:manualLayout>
@@ -1982,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E252F772-8BFF-4763-82E2-BAB23D65FFF3}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2095,20 +2095,20 @@
         <v>82591.6875</v>
       </c>
       <c r="G5" s="9">
-        <v>41088</v>
+        <v>34352</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ref="H5:H14" si="0">G5/F5</f>
-        <v>0.49748347858856862</v>
+        <v>0.41592563416263895</v>
       </c>
       <c r="J5" s="7">
         <v>10</v>
       </c>
       <c r="K5" s="9">
-        <v>0.49748347858856862</v>
+        <v>0.41592563416263895</v>
       </c>
       <c r="L5" s="9">
-        <v>0.20779247932833639</v>
+        <v>0.20435157350689198</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2129,20 +2129,20 @@
         <v>515188.1875</v>
       </c>
       <c r="G6" s="9">
-        <v>203476</v>
+        <v>175468</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" si="0"/>
-        <v>0.39495470769115798</v>
+        <v>0.34059010718292138</v>
       </c>
       <c r="J6" s="7">
         <v>20</v>
       </c>
       <c r="K6" s="9">
-        <v>0.39495470769115798</v>
+        <v>0.34059010718292138</v>
       </c>
       <c r="L6" s="9">
-        <v>0.19008113507889787</v>
+        <v>0.18903218651325307</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2163,20 +2163,20 @@
         <v>1556992.5</v>
       </c>
       <c r="G7" s="9">
-        <v>524532</v>
+        <v>462540</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" si="0"/>
-        <v>0.33688794262014748</v>
+        <v>0.2970727219302598</v>
       </c>
       <c r="J7" s="7">
         <v>30</v>
       </c>
       <c r="K7" s="9">
-        <v>0.33688794262014748</v>
+        <v>0.2970727219302598</v>
       </c>
       <c r="L7" s="9">
-        <v>0.19620276958603941</v>
+        <v>0.19505971752458229</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2197,20 +2197,20 @@
         <v>3448795</v>
       </c>
       <c r="G8" s="9">
-        <v>1083476</v>
+        <v>969068</v>
       </c>
       <c r="H8" s="9">
         <f t="shared" si="0"/>
-        <v>0.31416074310012626</v>
+        <v>0.28098741734431881</v>
       </c>
       <c r="J8" s="7">
         <v>40</v>
       </c>
       <c r="K8" s="9">
-        <v>0.31416074310012626</v>
+        <v>0.28098741734431881</v>
       </c>
       <c r="L8" s="9">
-        <v>0.19475661614713657</v>
+        <v>0.19418922833756871</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2231,20 +2231,20 @@
         <v>6432790</v>
       </c>
       <c r="G9" s="9">
-        <v>1895188</v>
+        <v>1715692</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" si="0"/>
-        <v>0.29461369017176064</v>
+        <v>0.26671040093023402</v>
       </c>
       <c r="J9" s="7">
         <v>50</v>
       </c>
       <c r="K9" s="9">
-        <v>0.29461369017176064</v>
+        <v>0.26671040093023402</v>
       </c>
       <c r="L9" s="9">
-        <v>0.19591126502897765</v>
+        <v>0.19532763977043302</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2265,20 +2265,20 @@
         <v>10793006</v>
       </c>
       <c r="G10" s="9">
-        <v>3009972</v>
+        <v>2753292</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>0.27888171284255747</v>
+        <v>0.25509964508497446</v>
       </c>
       <c r="J10" s="7">
         <v>60</v>
       </c>
       <c r="K10" s="9">
-        <v>0.27888171284255747</v>
+        <v>0.25509964508497446</v>
       </c>
       <c r="L10" s="9">
-        <v>0.19501287501118031</v>
+        <v>0.19471428504178578</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2299,20 +2299,20 @@
         <v>16966040</v>
       </c>
       <c r="G11" s="9">
-        <v>4496564</v>
+        <v>4145420</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" si="0"/>
-        <v>0.26503320751336201</v>
+        <v>0.24433633305120112</v>
       </c>
       <c r="J11" s="7">
         <v>70</v>
       </c>
       <c r="K11" s="9">
-        <v>0.26503320751336201</v>
+        <v>0.24433633305120112</v>
       </c>
       <c r="L11" s="9">
-        <v>0.19518225405811335</v>
+        <v>0.19480691115616602</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2333,20 +2333,20 @@
         <v>25109084</v>
       </c>
       <c r="G12" s="9">
-        <v>6404116</v>
+        <v>5942380</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>0.25505175736398827</v>
+        <v>0.23666255606934924</v>
       </c>
       <c r="J12" s="7">
         <v>80</v>
       </c>
       <c r="K12" s="9">
-        <v>0.25505175736398827</v>
+        <v>0.23666255606934924</v>
       </c>
       <c r="L12" s="9">
-        <v>0.19439825946692643</v>
+        <v>0.19408299736292856</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2367,20 +2367,20 @@
         <v>35401044</v>
       </c>
       <c r="G13" s="9">
-        <v>8725332</v>
+        <v>8145516</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
-        <v>0.24647103627791317</v>
+        <v>0.23009253625401557</v>
       </c>
       <c r="J13" s="7">
         <v>90</v>
       </c>
       <c r="K13" s="9">
-        <v>0.24647103627791317</v>
+        <v>0.23009253625401557</v>
       </c>
       <c r="L13" s="9">
-        <v>0.19491339731850818</v>
+        <v>0.19458412618878609</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -2401,20 +2401,20 @@
         <v>48375082</v>
       </c>
       <c r="G14" s="9">
-        <v>11608148</v>
+        <v>10886060</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="0"/>
-        <v>0.2399613090061532</v>
+        <v>0.22503445058759797</v>
       </c>
       <c r="J14" s="7">
         <v>100</v>
       </c>
       <c r="K14" s="9">
-        <v>0.2399613090061532</v>
+        <v>0.22503445058759797</v>
       </c>
       <c r="L14" s="9">
-        <v>0.19358716310804974</v>
+        <v>0.19334298037912881</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2524,11 +2524,11 @@
         <v>41849.4453125</v>
       </c>
       <c r="G21" s="9">
-        <v>8696</v>
+        <v>8552</v>
       </c>
       <c r="H21" s="9">
         <f t="shared" ref="H21:H30" si="3">G21/F21</f>
-        <v>0.20779247932833639</v>
+        <v>0.20435157350689198</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2549,11 +2549,11 @@
         <v>343200.8125</v>
       </c>
       <c r="G22" s="9">
-        <v>65236</v>
+        <v>64876</v>
       </c>
       <c r="H22" s="9">
         <f t="shared" si="3"/>
-        <v>0.19008113507889787</v>
+        <v>0.18903218651325307</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2574,11 +2574,11 @@
         <v>1133806.625</v>
       </c>
       <c r="G23" s="9">
-        <v>222456</v>
+        <v>221160</v>
       </c>
       <c r="H23" s="9">
         <f t="shared" si="3"/>
-        <v>0.19620276958603941</v>
+        <v>0.19505971752458229</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2599,11 +2599,11 @@
         <v>2664844</v>
       </c>
       <c r="G24" s="9">
-        <v>518996</v>
+        <v>517484</v>
       </c>
       <c r="H24" s="9">
         <f t="shared" si="3"/>
-        <v>0.19475661614713657</v>
+        <v>0.19418922833756871</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2624,11 +2624,11 @@
         <v>5181407</v>
       </c>
       <c r="G25" s="9">
-        <v>1015096</v>
+        <v>1012072</v>
       </c>
       <c r="H25" s="9">
         <f t="shared" si="3"/>
-        <v>0.19591126502897765</v>
+        <v>0.19532763977043302</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -2649,11 +2649,11 @@
         <v>8921934</v>
       </c>
       <c r="G26" s="9">
-        <v>1739892</v>
+        <v>1737228</v>
       </c>
       <c r="H26" s="9">
         <f t="shared" si="3"/>
-        <v>0.19501287501118031</v>
+        <v>0.19471428504178578</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2664,11 +2664,11 @@
         <v>14195020</v>
       </c>
       <c r="G27" s="9">
-        <v>2770616</v>
+        <v>2765288</v>
       </c>
       <c r="H27" s="9">
         <f t="shared" si="3"/>
-        <v>0.19518225405811335</v>
+        <v>0.19480691115616602</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2679,11 +2679,11 @@
         <v>21239470</v>
       </c>
       <c r="G28" s="9">
-        <v>4128916</v>
+        <v>4122220</v>
       </c>
       <c r="H28" s="9">
         <f t="shared" si="3"/>
-        <v>0.19439825946692643</v>
+        <v>0.19408299736292856</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2694,11 +2694,11 @@
         <v>30175740</v>
       </c>
       <c r="G29" s="9">
-        <v>5881656</v>
+        <v>5871720</v>
       </c>
       <c r="H29" s="9">
         <f t="shared" si="3"/>
-        <v>0.19491339731850818</v>
+        <v>0.19458412618878609</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2709,11 +2709,11 @@
         <v>41575422</v>
       </c>
       <c r="G30" s="9">
-        <v>8048468</v>
+        <v>8038316</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="3"/>
-        <v>0.19358716310804974</v>
+        <v>0.19334298037912881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a mistake when counting adds in polygonise
</commit_message>
<xml_diff>
--- a/Data/baseline_timing.xlsx
+++ b/Data/baseline_timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eth\asl\team42\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B730ACD3-6AEF-4892-AF01-6FCF25015E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCD183F-1455-43EE-A7C9-3C4EACAB3D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1F9DB3D-A5ED-4CF3-8993-B9AA5F6B7807}"/>
   </bookViews>
@@ -547,34 +547,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.41592563416263895</c:v>
+                  <c:v>0.37262829870136749</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34059010718292138</c:v>
+                  <c:v>0.31310500495510679</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2970727219302598</c:v>
+                  <c:v>0.27687994643519476</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28098741734431881</c:v>
+                  <c:v>0.26435552127627188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26671040093023402</c:v>
+                  <c:v>0.2526449643156391</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25509964508497446</c:v>
+                  <c:v>0.24316747345456863</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24433633305120112</c:v>
+                  <c:v>0.23392777572138224</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23666255606934924</c:v>
+                  <c:v>0.22746174253110946</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23009253625401557</c:v>
+                  <c:v>0.2218500674725864</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22503445058759797</c:v>
+                  <c:v>0.21755588962102432</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,34 +670,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.20435157350689198</c:v>
+                  <c:v>0.20320460489974385</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18903218651325307</c:v>
+                  <c:v>0.18805316785198462</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19505971752458229</c:v>
+                  <c:v>0.19450935912462144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19418922833756871</c:v>
+                  <c:v>0.19384699442068654</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19532763977043302</c:v>
+                  <c:v>0.19504045908765708</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.19471428504178578</c:v>
+                  <c:v>0.19451522506218943</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.19480691115616602</c:v>
+                  <c:v>0.19462093043898493</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.19408299736292856</c:v>
+                  <c:v>0.19391802149488666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.19458412618878609</c:v>
+                  <c:v>0.19442028596481808</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19334298037912881</c:v>
+                  <c:v>0.19320328245856411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,12 +996,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1982,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E252F772-8BFF-4763-82E2-BAB23D65FFF3}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L14"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2095,20 +2090,20 @@
         <v>82591.6875</v>
       </c>
       <c r="G5" s="9">
-        <v>34352</v>
+        <v>30776</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ref="H5:H14" si="0">G5/F5</f>
-        <v>0.41592563416263895</v>
+        <v>0.37262829870136749</v>
       </c>
       <c r="J5" s="7">
         <v>10</v>
       </c>
       <c r="K5" s="9">
-        <v>0.41592563416263895</v>
+        <v>0.37262829870136749</v>
       </c>
       <c r="L5" s="9">
-        <v>0.20435157350689198</v>
+        <v>0.20320460489974385</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2129,20 +2124,20 @@
         <v>515188.1875</v>
       </c>
       <c r="G6" s="9">
-        <v>175468</v>
+        <v>161308</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" si="0"/>
-        <v>0.34059010718292138</v>
+        <v>0.31310500495510679</v>
       </c>
       <c r="J6" s="7">
         <v>20</v>
       </c>
       <c r="K6" s="9">
-        <v>0.34059010718292138</v>
+        <v>0.31310500495510679</v>
       </c>
       <c r="L6" s="9">
-        <v>0.18903218651325307</v>
+        <v>0.18805316785198462</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2163,20 +2158,20 @@
         <v>1556992.5</v>
       </c>
       <c r="G7" s="9">
-        <v>462540</v>
+        <v>431100</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" si="0"/>
-        <v>0.2970727219302598</v>
+        <v>0.27687994643519476</v>
       </c>
       <c r="J7" s="7">
         <v>30</v>
       </c>
       <c r="K7" s="9">
-        <v>0.2970727219302598</v>
+        <v>0.27687994643519476</v>
       </c>
       <c r="L7" s="9">
-        <v>0.19505971752458229</v>
+        <v>0.19450935912462144</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2197,20 +2192,20 @@
         <v>3448795</v>
       </c>
       <c r="G8" s="9">
-        <v>969068</v>
+        <v>911708</v>
       </c>
       <c r="H8" s="9">
         <f t="shared" si="0"/>
-        <v>0.28098741734431881</v>
+        <v>0.26435552127627188</v>
       </c>
       <c r="J8" s="7">
         <v>40</v>
       </c>
       <c r="K8" s="9">
-        <v>0.28098741734431881</v>
+        <v>0.26435552127627188</v>
       </c>
       <c r="L8" s="9">
-        <v>0.19418922833756871</v>
+        <v>0.19384699442068654</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2231,20 +2226,20 @@
         <v>6432790</v>
       </c>
       <c r="G9" s="9">
-        <v>1715692</v>
+        <v>1625212</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" si="0"/>
-        <v>0.26671040093023402</v>
+        <v>0.2526449643156391</v>
       </c>
       <c r="J9" s="7">
         <v>50</v>
       </c>
       <c r="K9" s="9">
-        <v>0.26671040093023402</v>
+        <v>0.2526449643156391</v>
       </c>
       <c r="L9" s="9">
-        <v>0.19532763977043302</v>
+        <v>0.19504045908765708</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2265,20 +2260,20 @@
         <v>10793006</v>
       </c>
       <c r="G10" s="9">
-        <v>2753292</v>
+        <v>2624508</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>0.25509964508497446</v>
+        <v>0.24316747345456863</v>
       </c>
       <c r="J10" s="7">
         <v>60</v>
       </c>
       <c r="K10" s="9">
-        <v>0.25509964508497446</v>
+        <v>0.24316747345456863</v>
       </c>
       <c r="L10" s="9">
-        <v>0.19471428504178578</v>
+        <v>0.19451522506218943</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2299,20 +2294,20 @@
         <v>16966040</v>
       </c>
       <c r="G11" s="9">
-        <v>4145420</v>
+        <v>3968828</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" si="0"/>
-        <v>0.24433633305120112</v>
+        <v>0.23392777572138224</v>
       </c>
       <c r="J11" s="7">
         <v>70</v>
       </c>
       <c r="K11" s="9">
-        <v>0.24433633305120112</v>
+        <v>0.23392777572138224</v>
       </c>
       <c r="L11" s="9">
-        <v>0.19480691115616602</v>
+        <v>0.19462093043898493</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2333,20 +2328,20 @@
         <v>25109084</v>
       </c>
       <c r="G12" s="9">
-        <v>5942380</v>
+        <v>5711356</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>0.23666255606934924</v>
+        <v>0.22746174253110946</v>
       </c>
       <c r="J12" s="7">
         <v>80</v>
       </c>
       <c r="K12" s="9">
-        <v>0.23666255606934924</v>
+        <v>0.22746174253110946</v>
       </c>
       <c r="L12" s="9">
-        <v>0.19408299736292856</v>
+        <v>0.19391802149488666</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2367,20 +2362,20 @@
         <v>35401044</v>
       </c>
       <c r="G13" s="9">
-        <v>8145516</v>
+        <v>7853724</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
-        <v>0.23009253625401557</v>
+        <v>0.2218500674725864</v>
       </c>
       <c r="J13" s="7">
         <v>90</v>
       </c>
       <c r="K13" s="9">
-        <v>0.23009253625401557</v>
+        <v>0.2218500674725864</v>
       </c>
       <c r="L13" s="9">
-        <v>0.19458412618878609</v>
+        <v>0.19442028596481808</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -2401,20 +2396,20 @@
         <v>48375082</v>
       </c>
       <c r="G14" s="9">
-        <v>10886060</v>
+        <v>10524284</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="0"/>
-        <v>0.22503445058759797</v>
+        <v>0.21755588962102432</v>
       </c>
       <c r="J14" s="7">
         <v>100</v>
       </c>
       <c r="K14" s="9">
-        <v>0.22503445058759797</v>
+        <v>0.21755588962102432</v>
       </c>
       <c r="L14" s="9">
-        <v>0.19334298037912881</v>
+        <v>0.19320328245856411</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2524,11 +2519,11 @@
         <v>41849.4453125</v>
       </c>
       <c r="G21" s="9">
-        <v>8552</v>
+        <v>8504</v>
       </c>
       <c r="H21" s="9">
         <f t="shared" ref="H21:H30" si="3">G21/F21</f>
-        <v>0.20435157350689198</v>
+        <v>0.20320460489974385</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2549,11 +2544,11 @@
         <v>343200.8125</v>
       </c>
       <c r="G22" s="9">
-        <v>64876</v>
+        <v>64540</v>
       </c>
       <c r="H22" s="9">
         <f t="shared" si="3"/>
-        <v>0.18903218651325307</v>
+        <v>0.18805316785198462</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2574,11 +2569,11 @@
         <v>1133806.625</v>
       </c>
       <c r="G23" s="9">
-        <v>221160</v>
+        <v>220536</v>
       </c>
       <c r="H23" s="9">
         <f t="shared" si="3"/>
-        <v>0.19505971752458229</v>
+        <v>0.19450935912462144</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2599,11 +2594,11 @@
         <v>2664844</v>
       </c>
       <c r="G24" s="9">
-        <v>517484</v>
+        <v>516572</v>
       </c>
       <c r="H24" s="9">
         <f t="shared" si="3"/>
-        <v>0.19418922833756871</v>
+        <v>0.19384699442068654</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2624,11 +2619,11 @@
         <v>5181407</v>
       </c>
       <c r="G25" s="9">
-        <v>1012072</v>
+        <v>1010584</v>
       </c>
       <c r="H25" s="9">
         <f t="shared" si="3"/>
-        <v>0.19532763977043302</v>
+        <v>0.19504045908765708</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -2649,11 +2644,11 @@
         <v>8921934</v>
       </c>
       <c r="G26" s="9">
-        <v>1737228</v>
+        <v>1735452</v>
       </c>
       <c r="H26" s="9">
         <f t="shared" si="3"/>
-        <v>0.19471428504178578</v>
+        <v>0.19451522506218943</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2664,11 +2659,11 @@
         <v>14195020</v>
       </c>
       <c r="G27" s="9">
-        <v>2765288</v>
+        <v>2762648</v>
       </c>
       <c r="H27" s="9">
         <f t="shared" si="3"/>
-        <v>0.19480691115616602</v>
+        <v>0.19462093043898493</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2679,11 +2674,11 @@
         <v>21239470</v>
       </c>
       <c r="G28" s="9">
-        <v>4122220</v>
+        <v>4118716</v>
       </c>
       <c r="H28" s="9">
         <f t="shared" si="3"/>
-        <v>0.19408299736292856</v>
+        <v>0.19391802149488666</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2694,11 +2689,11 @@
         <v>30175740</v>
       </c>
       <c r="G29" s="9">
-        <v>5871720</v>
+        <v>5866776</v>
       </c>
       <c r="H29" s="9">
         <f t="shared" si="3"/>
-        <v>0.19458412618878609</v>
+        <v>0.19442028596481808</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2709,11 +2704,11 @@
         <v>41575422</v>
       </c>
       <c r="G30" s="9">
-        <v>8038316</v>
+        <v>8032508</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="3"/>
-        <v>0.19334298037912881</v>
+        <v>0.19320328245856411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>